<commit_message>
updated hours on Master Gantt
</commit_message>
<xml_diff>
--- a/doc/Master_Gantt.xlsx
+++ b/doc/Master_Gantt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\travi\Desktop\Team-Faucet\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Hill\Documents\GitHub\Team-Faucet\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD89C239-E868-4CF6-B624-AB3940CBB3E5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{24327E33-5E17-41B8-A917-F1E518100254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -29,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Travis Rousey</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{C385386C-B8E9-4EFA-A685-26BE3A2D6F61}">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -476,7 +475,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -4610,11 +4609,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33873E7D-5C5F-4C76-AC1C-D81FEE5D415F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7987,7 +7986,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1" xr:uid="{7B565046-8104-402B-AE5E-61CA7E420F59}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1">
       <formula1>personList</formula1>
     </dataValidation>
   </dataValidations>
@@ -7999,11 +7998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E405C95B-F562-491A-BE4E-D61A355ABBB1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8360,6 +8359,9 @@
       <c r="B43">
         <v>10</v>
       </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
@@ -8368,6 +8370,9 @@
       <c r="B44">
         <v>7</v>
       </c>
+      <c r="C44">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
@@ -8376,6 +8381,9 @@
       <c r="B45">
         <v>7</v>
       </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
@@ -8383,6 +8391,9 @@
       </c>
       <c r="B46">
         <v>7</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -8781,7 +8792,7 @@
       </c>
       <c r="C92">
         <f>SUM(C2:C90)</f>
-        <v>49.5</v>
+        <v>68</v>
       </c>
       <c r="D92" s="8">
         <f>B92*100</f>
@@ -8789,7 +8800,7 @@
       </c>
       <c r="E92" s="8">
         <f>C92*100</f>
-        <v>4950</v>
+        <v>6800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Gantt and moved cs files
</commit_message>
<xml_diff>
--- a/doc/Master_Gantt.xlsx
+++ b/doc/Master_Gantt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Hill\Documents\GitHub\Team-Faucet\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\travi\Desktop\Team-Faucet\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EE6BD6-AF02-4722-B2EE-C03D7FF99B7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="personList">Gantt!$B$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Travis Rousey</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="137">
   <si>
     <t>Persons</t>
   </si>
@@ -331,15 +332,6 @@
     <t>Create test Items</t>
   </si>
   <si>
-    <t>Create giveitemtoplayer()</t>
-  </si>
-  <si>
-    <t>Create enemydropitem()</t>
-  </si>
-  <si>
-    <t>Create chestdropitem()</t>
-  </si>
-  <si>
     <t>Create all necessary items</t>
   </si>
   <si>
@@ -470,12 +462,24 @@
   </si>
   <si>
     <t>Zane</t>
+  </si>
+  <si>
+    <t>Make items stack/swap</t>
+  </si>
+  <si>
+    <t>Integrate Inventory into the main game</t>
+  </si>
+  <si>
+    <t>Make item objects in game move to inventory</t>
+  </si>
+  <si>
+    <t>Integrate Inventory into the main game (4/12/2018)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -941,7 +945,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Zane G.</c:v>
+              <c:v>Travis R.</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -991,7 +995,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Zane G.</c:v>
+                  <c:v>Travis R.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1017,28 +1021,28 @@
                   <c:v>Documentation/SA demo</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Outline Manager and Functions</c:v>
+                  <c:v>Create Inventory</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Build Sound Library</c:v>
+                  <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Working Functions for all possible audio requests</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Algorithm for dynamic pitch of sounds</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Modify sounds/music for optimal load times</c:v>
+                  <c:v>Testing</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Create all necessary items</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Presentation</c:v>
+                  <c:v>Final Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1056,13 +1060,13 @@
                   <c:v>43143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43150</c:v>
+                  <c:v>43157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43171</c:v>
+                  <c:v>43164</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43185</c:v>
+                  <c:v>43178</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43192</c:v>
@@ -1071,10 +1075,10 @@
                   <c:v>43206</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>43213</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>43220</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1118,28 +1122,28 @@
                   <c:v>Documentation/SA demo</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Outline Manager and Functions</c:v>
+                  <c:v>Create Inventory</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Build Sound Library</c:v>
+                  <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Working Functions for all possible audio requests</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Algorithm for dynamic pitch of sounds</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Modify sounds/music for optimal load times</c:v>
+                  <c:v>Testing</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Create all necessary items</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Presentation</c:v>
+                  <c:v>Final Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1154,16 +1158,16 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1219,28 +1223,28 @@
                   <c:v>Documentation/SA demo</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Outline Manager and Functions</c:v>
+                  <c:v>Create Inventory</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Build Sound Library</c:v>
+                  <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Working Functions for all possible audio requests</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Algorithm for dynamic pitch of sounds</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Modify sounds/music for optimal load times</c:v>
+                  <c:v>Testing</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Testing/Debugging</c:v>
+                  <c:v>Create all necessary items</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Presentation</c:v>
+                  <c:v>Final Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1261,22 +1265,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1669,13 +1673,13 @@
                   <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>Create giveitemtoplayer()</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>Create enemydropitem()</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>Create chestdropitem()</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>Testing</c:v>
@@ -2164,13 +2168,13 @@
                   <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>Create giveitemtoplayer()</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>Create enemydropitem()</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>Create chestdropitem()</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>Testing</c:v>
@@ -2401,10 +2405,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>0</c:v>
@@ -2659,13 +2663,13 @@
                   <c:v>Create test Items</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>Create giveitemtoplayer()</c:v>
+                  <c:v>Make items stack/swap</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>Create enemydropitem()</c:v>
+                  <c:v>Integrate Inventory into the main game</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>Create chestdropitem()</c:v>
+                  <c:v>Make item objects in game move to inventory</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>Testing</c:v>
@@ -2896,10 +2900,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>14</c:v>
@@ -4609,11 +4613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4667,7 +4671,7 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4720,16 +4724,16 @@
         <v>64</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>87</v>
@@ -4745,7 +4749,7 @@
       </c>
       <c r="L3" s="5" t="str">
         <f>HLOOKUP($L$1,$B$1:$J$46,K3,FALSE)</f>
-        <v>Outline Manager and Functions</v>
+        <v>Create Inventory</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4759,16 +4763,16 @@
         <v>65</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>88</v>
@@ -4784,7 +4788,7 @@
       </c>
       <c r="L4" s="5" t="str">
         <f t="shared" ref="L4:L46" si="0">HLOOKUP($L$1,$B$1:$J$46,K4,FALSE)</f>
-        <v>Build Sound Library</v>
+        <v>Create test Items</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4798,19 +4802,19 @@
         <v>66</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>82</v>
@@ -4823,7 +4827,7 @@
       </c>
       <c r="L5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Working Functions for all possible audio requests</v>
+        <v>Make items stack/swap</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4837,19 +4841,19 @@
         <v>67</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>83</v>
@@ -4862,7 +4866,7 @@
       </c>
       <c r="L6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Testing/Debugging</v>
+        <v>Integrate Inventory into the main game</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4876,19 +4880,19 @@
         <v>68</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>84</v>
@@ -4901,7 +4905,7 @@
       </c>
       <c r="L7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Algorithm for dynamic pitch of sounds</v>
+        <v>Make item objects in game move to inventory</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4915,16 +4919,16 @@
         <v>69</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>70</v>
@@ -4940,7 +4944,7 @@
       </c>
       <c r="L8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Modify sounds/music for optimal load times</v>
+        <v>Testing</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4960,13 +4964,13 @@
         <v>70</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>70</v>
@@ -4979,7 +4983,7 @@
       </c>
       <c r="L9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Testing/Debugging</v>
+        <v>Create all necessary items</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4996,7 +5000,7 @@
         <v>79</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>79</v>
@@ -5005,7 +5009,7 @@
         <v>79</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>86</v>
@@ -5018,7 +5022,7 @@
       </c>
       <c r="L10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Presentation</v>
+        <v>Final Testing</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -5135,7 +5139,7 @@
       </c>
       <c r="L13" s="6">
         <f t="shared" si="0"/>
-        <v>43150</v>
+        <v>43157</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -5174,7 +5178,7 @@
       </c>
       <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>43171</v>
+        <v>43164</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -5213,7 +5217,7 @@
       </c>
       <c r="L15" s="6">
         <f t="shared" si="0"/>
-        <v>43185</v>
+        <v>43178</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -5330,7 +5334,7 @@
       </c>
       <c r="L18" s="6">
         <f t="shared" si="0"/>
-        <v>43220</v>
+        <v>43213</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5369,7 +5373,7 @@
       </c>
       <c r="L19" s="6">
         <f t="shared" si="0"/>
-        <v>43223</v>
+        <v>43220</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -5447,7 +5451,7 @@
       </c>
       <c r="L21" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -5486,7 +5490,7 @@
       </c>
       <c r="L22" s="5">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -5528,7 +5532,7 @@
         <v>14</v>
       </c>
       <c r="M23" s="23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -5567,7 +5571,7 @@
       </c>
       <c r="L24" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M24" s="24"/>
     </row>
@@ -5647,7 +5651,7 @@
       </c>
       <c r="L26" s="22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="M26" s="25"/>
     </row>
@@ -5687,7 +5691,7 @@
       </c>
       <c r="L27" s="22">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M27" s="25"/>
     </row>
@@ -5727,7 +5731,7 @@
       </c>
       <c r="L28" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M28" s="25"/>
     </row>
@@ -5807,7 +5811,7 @@
       </c>
       <c r="L30" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M30" s="25"/>
     </row>
@@ -5847,10 +5851,10 @@
       </c>
       <c r="L31" s="22">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="M31" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -5876,7 +5880,7 @@
         <v>14</v>
       </c>
       <c r="H32" s="30">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I32" s="30">
         <v>14</v>
@@ -5889,7 +5893,7 @@
       </c>
       <c r="L32" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M32" s="25"/>
     </row>
@@ -5916,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="30">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I33" s="30">
         <v>0</v>
@@ -5929,7 +5933,7 @@
       </c>
       <c r="L33" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M33" s="25"/>
     </row>
@@ -6141,7 +6145,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -6272,7 +6276,7 @@
       </c>
       <c r="H41" s="28">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I41" s="28">
         <f t="shared" si="2"/>
@@ -6287,7 +6291,7 @@
       </c>
       <c r="L41" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M41" s="25"/>
     </row>
@@ -6321,7 +6325,7 @@
       </c>
       <c r="H42" s="28">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I42" s="28">
         <f t="shared" si="2"/>
@@ -6336,7 +6340,7 @@
       </c>
       <c r="L42" s="22">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M42" s="25"/>
     </row>
@@ -6434,7 +6438,7 @@
       </c>
       <c r="L44" s="22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="M44" s="25"/>
     </row>
@@ -6483,7 +6487,7 @@
       </c>
       <c r="L45" s="22">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M45" s="26"/>
     </row>
@@ -6532,10 +6536,10 @@
       </c>
       <c r="L46" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M46" s="25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -6544,7 +6548,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C48" s="27">
         <f>B11</f>
@@ -6639,7 +6643,7 @@
         <v>14</v>
       </c>
       <c r="M52" s="25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
@@ -6720,7 +6724,7 @@
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C57" s="3">
         <f>C11</f>
@@ -6758,7 +6762,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
@@ -6893,12 +6897,12 @@
         <v>3</v>
       </c>
       <c r="M65" s="25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C66" s="4">
         <f>D11</f>
@@ -7012,7 +7016,7 @@
         <v>14</v>
       </c>
       <c r="M71" s="25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
@@ -7074,7 +7078,7 @@
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C75" s="4">
         <f>E11</f>
@@ -7131,7 +7135,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
@@ -7231,7 +7235,7 @@
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C83" s="4">
         <f>F11</f>
@@ -7380,7 +7384,7 @@
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B91" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C91" s="4">
         <f>G11</f>
@@ -7527,7 +7531,7 @@
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C99" s="4">
         <f>H11</f>
@@ -7589,15 +7593,15 @@
       </c>
       <c r="D102" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>Create giveitemtoplayer()</v>
+        <v>Make items stack/swap</v>
       </c>
       <c r="E102">
         <f t="shared" si="29"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F102" s="7">
         <f t="shared" si="30"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -7607,15 +7611,15 @@
       </c>
       <c r="D103" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>Create enemydropitem()</v>
+        <v>Integrate Inventory into the main game</v>
       </c>
       <c r="E103">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F103" s="7">
         <f t="shared" si="30"/>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -7625,7 +7629,7 @@
       </c>
       <c r="D104" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>Create chestdropitem()</v>
+        <v>Make item objects in game move to inventory</v>
       </c>
       <c r="E104">
         <f t="shared" si="29"/>
@@ -7674,7 +7678,7 @@
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C107" s="4">
         <f>I11</f>
@@ -7821,7 +7825,7 @@
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C115" s="4">
         <f>J11</f>
@@ -7986,7 +7990,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>personList</formula1>
     </dataValidation>
   </dataValidations>
@@ -7998,11 +8002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8019,10 +8023,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8193,7 +8197,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -8201,7 +8205,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -8209,7 +8213,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -8217,7 +8221,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -8225,7 +8229,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -8233,7 +8237,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -8272,7 +8276,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B33">
         <v>5</v>
@@ -8280,7 +8284,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -8288,7 +8292,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -8296,7 +8300,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -8304,7 +8308,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B37">
         <v>5</v>
@@ -8312,7 +8316,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -8328,7 +8332,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -8354,7 +8358,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B43">
         <v>10</v>
@@ -8365,7 +8369,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B44">
         <v>7</v>
@@ -8376,7 +8380,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B45">
         <v>7</v>
@@ -8387,7 +8391,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B46">
         <v>7</v>
@@ -8398,7 +8402,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -8406,7 +8410,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B48">
         <v>6</v>
@@ -8414,7 +8418,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -8445,7 +8449,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -8453,7 +8457,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -8461,7 +8465,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -8469,7 +8473,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -8477,7 +8481,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -8485,7 +8489,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -8493,7 +8497,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -8549,29 +8553,29 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B65">
         <v>5</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="B66">
         <v>5</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="B67">
         <v>5</v>
@@ -8593,7 +8597,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -8604,7 +8608,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -8773,16 +8777,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" s="20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -8792,7 +8796,7 @@
       </c>
       <c r="C92">
         <f>SUM(C2:C90)</f>
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D92" s="8">
         <f>B92*100</f>
@@ -8800,7 +8804,7 @@
       </c>
       <c r="E92" s="8">
         <f>C92*100</f>
-        <v>6800</v>
+        <v>8700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>